<commit_message>
added multi task types
</commit_message>
<xml_diff>
--- a/files/file.xlsx
+++ b/files/file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Название анкеты</t>
   </si>
@@ -40,7 +40,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Анкета №4</t>
+    <t xml:space="preserve">Анкета - Визит к ЛПР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 16</t>
   </si>
   <si>
     <t>Заголовок</t>
@@ -91,28 +94,91 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Основная информация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Укажите возраст</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Укажите пол</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мужской, Женский</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дополнительная информация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Укажите профессию</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Есть ли дети?</t>
+    <t xml:space="preserve">Подготовка к визиту</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.SMART-Цель на данный визит согласно истории развития клиента и ЛПУ и результатам предыдущего визита.</t>
   </si>
   <si>
     <t xml:space="preserve">Да, Нет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Получена вся необходимая информация для визита (потребность отделений, расход препарата и фарм.группы за месяц, медицинская и фармако-экономическая информация, финансирование и т.д.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Открытие визита </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Контакт с ЛПР установлен.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.Выявлен опыт применения препарата, МНН, фарм.группы в ЛПУ и договоренности</t>
+  </si>
+  <si>
+    <t>Диагностика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Потребность ЛПУ в препаратах ИФ и конкурентах из категории</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Текущая ситуация (закуп - уходимость препаратов ИФ и конкурентов, бюджет)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Сдерживающие/cтимулирующие факторы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Сроки и периодичность заявки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Презентация </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Презентация преимуществ применения  фокусных препаратов ИФ для ЛПУ с использованием выявленной потребности и необходимых аргументов (медицинских, фармако-экономических)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Маркетинговая стратегия </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Донесение на визите Ключевого сообщения по фокусному препарату согласно маркетинговой сетке</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Реакция на презентацию</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Реакция на презентацию отработана</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.Негативные реакции и возражения сняты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завершение визита</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Получено измеримое (количество/доля) подтверждение по закупу, согласно Цели визита, определены сроки закупки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.Предпочтения по поставщикам </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Имеется пошаговый план реализации закупа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Подведен итог </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Анализ визита</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Выполнение поставленной Цели.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.Результаты визита зафиксированы.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.Цель (SMART) на следующий визит поставлена по результатам данного визита. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.План развития клиента, ЛПУ</t>
   </si>
 </sst>
 </file>
@@ -154,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,10 +228,12 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,8 +763,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>4</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -716,77 +784,305 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.57421875"/>
-    <col customWidth="1" min="2" max="2" width="22.140625"/>
+    <col customWidth="1" min="1" max="2" width="32.57421875"/>
     <col customWidth="1" min="3" max="3" width="36.421875"/>
     <col customWidth="1" min="4" max="4" width="40.8515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="46.799999999999997" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="171">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
+      <c r="A4" t="s">
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25"/>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>